<commit_message>
fix product UTF8 encodage
</commit_message>
<xml_diff>
--- a/Excel/products.xlsx
+++ b/Excel/products.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugo/Desktop/school-uni-bd6/Excel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC60E63-049D-B343-9728-A7D7DE5EEF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="13480" windowHeight="19120" xr2:uid="{CEC91E52-384D-4B86-A26F-F5C7632966B9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="13480" windowHeight="14620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -58,9 +52,6 @@
     <t>Rhum</t>
   </si>
   <si>
-    <t>Bière</t>
-  </si>
-  <si>
     <t>Riz</t>
   </si>
   <si>
@@ -91,9 +82,6 @@
     <t>YES</t>
   </si>
   <si>
-    <t>Blé</t>
-  </si>
-  <si>
     <t>Saucisse</t>
   </si>
   <si>
@@ -121,28 +109,34 @@
     <t>Bottes de marin</t>
   </si>
   <si>
-    <t>Montre à gousset</t>
-  </si>
-  <si>
     <t>Verre</t>
   </si>
   <si>
     <t>Sable</t>
   </si>
   <si>
-    <t>Vêtements de travailleur</t>
-  </si>
-  <si>
     <t>Collier en or</t>
   </si>
   <si>
-    <t>Viande séchée</t>
+    <t>Vetements de travailleur</t>
+  </si>
+  <si>
+    <t>Biere</t>
+  </si>
+  <si>
+    <t>Montre a gousset</t>
+  </si>
+  <si>
+    <t>Ble</t>
+  </si>
+  <si>
+    <t>Viande sechee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -480,26 +474,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF94A26-5CE8-4938-A8A0-A764AC925EA4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,12 +507,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -527,7 +521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -538,15 +532,15 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -555,12 +549,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -569,12 +563,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -583,40 +577,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>40</v>
@@ -625,12 +619,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -639,12 +633,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>120</v>
@@ -653,12 +647,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -667,12 +661,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>40</v>
@@ -681,12 +675,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>20</v>
@@ -695,12 +689,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -709,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -723,12 +717,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -737,12 +731,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -751,12 +745,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -765,12 +759,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -779,12 +773,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C21">
         <v>30</v>
@@ -793,12 +787,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>40</v>
@@ -807,12 +801,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -821,12 +815,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24">
         <v>10</v>
@@ -835,26 +829,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25">
         <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -863,35 +857,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C27">
         <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28">
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -902,7 +896,7 @@
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>